<commit_message>
Online Learning - Lihat Modul
</commit_message>
<xml_diff>
--- a/Data Binding.xlsx
+++ b/Data Binding.xlsx
@@ -8,12 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\git\LearningManagementWeb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDD31E57-262D-4ED4-9E8E-F2577337DC78}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{372BE063-6B36-417F-AE07-6CEC7842764C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{1D0504FE-B408-44BD-A9E7-7F1F2ED7EF33}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{1D0504FE-B408-44BD-A9E7-7F1F2ED7EF33}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="search" sheetId="1" r:id="rId1"/>
+    <sheet name="next page" sheetId="5" r:id="rId2"/>
+    <sheet name="lihat modul" sheetId="2" r:id="rId3"/>
+    <sheet name="materi belajar" sheetId="4" r:id="rId4"/>
+    <sheet name="review" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="16">
   <si>
     <t>search module</t>
   </si>
@@ -51,6 +55,36 @@
   </si>
   <si>
     <t>WELCOMING KIT</t>
+  </si>
+  <si>
+    <t>module_name</t>
+  </si>
+  <si>
+    <t>found</t>
+  </si>
+  <si>
+    <t>zzzzzzzzzz</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>yyyyyyyyyyy</t>
+  </si>
+  <si>
+    <t>NEOP AAV</t>
+  </si>
+  <si>
+    <t>review empty</t>
+  </si>
+  <si>
+    <t>new</t>
   </si>
 </sst>
 </file>
@@ -404,8 +438,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05FEBD06-F112-4A90-954F-2B4BBE3B5C42}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -440,4 +474,193 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33EBCB07-6B4E-4DCC-A2ED-2A237A435B8A}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23E6D39A-8162-48C0-8444-8140DAD53E39}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9802280-7071-47D4-AA4D-EEA7DD9C2C97}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7172DBA-6075-466A-AC8F-92175A2CE995}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>